<commit_message>
#691 office2016 excel 01 画像編集
</commit_message>
<xml_diff>
--- a/excel/03/population.xlsx
+++ b/excel/03/population.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hisashi/src/github.com/hatak/infolit/contents/office2013/excel/03/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="880" windowWidth="14960" windowHeight="12120"/>
+    <workbookView xWindow="975" yWindow="870" windowWidth="14955" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,15 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$I$50</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -369,6 +356,19 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>平成17年</t>
+    <rPh sb="0" eb="1">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>シゲル</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ネン</t>
+    </rPh>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
     <t>ほっかいどう</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -421,6 +421,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>人口、人口増減（平成12年～17年）、面積及び人口密度</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>かながわけん</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -554,6 +558,10 @@
   </si>
   <si>
     <t>おきなわけん</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>平成12年</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -650,37 +658,15 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
-  <si>
-    <t>人口、人口増減（平成22年～27年）、面積及び人口密度</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>平成27年</t>
-    <rPh sb="0" eb="1">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>シゲル</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ネン</t>
-    </rPh>
-    <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>平成22年</t>
-    <phoneticPr fontId="2"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="##,###,###,##0.0;&quot;-&quot;#,###,###,##0.0"/>
-    <numFmt numFmtId="177" formatCode="0.0_ "/>
+  <numFmts count="1">
+    <numFmt numFmtId="182" formatCode="##,###,###,##0.0;&quot;-&quot;#,###,###,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -731,253 +717,253 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -985,38 +971,38 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1027,7 +1013,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1091,20 +1077,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1123,431 +1100,337 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>76201</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1358900</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="7534274" cy="1438275"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1031" name="テキスト ボックス 1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
+        <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+        <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="9423400"/>
-          <a:ext cx="7518400" cy="1485900"/>
+          <a:off x="76201" y="9077324"/>
+          <a:ext cx="7534274" cy="1438275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="A3C4FF"/>
-            </a:gs>
-            <a:gs pos="35001">
-              <a:srgbClr val="BFD5FF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="E5EEFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="37999"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>注</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>) </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>国勢調査令（昭和</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>55</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>年政令第</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>98</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>号）の規定に基づき，調査の対象から</a:t>
+            <a:t>号）の規定に基づき，調査の対象から 除外された次の地域の面積を除いて算出した。</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
-            </a:rPr>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
             <a:t> </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>除外された次の地域の面積を除いて算出した。</a:t>
+            <a:t>　　 ａ　歯舞群島</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
-            </a:rPr>
-            <a:t>　　</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
-            </a:rPr>
-            <a:t>ａ　歯舞群島</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>(99.94km2)</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
-            </a:rPr>
+            <a:rPr lang="en-US" altLang="ja-JP"/>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>　　ｂ　色丹島</a:t>
+            <a:t>　　ｂ　色丹島* </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>* (253.33km2)</a:t>
+            <a:t>(253.33km2)</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>，国後島</a:t>
+            <a:t>，国後島* </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>* (1498.83km2)</a:t>
+            <a:t>(1498.83km2)</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>及び択捉島</a:t>
+            <a:t>及び択捉島*</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>*(3184.04km2) (*</a:t>
+            <a:t>(3184.04km2) (*</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>属島を含む</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>)</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
-            </a:rPr>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>　　ｃ　竹島</a:t>
+            <a:t>　　ｃ　竹島 </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> (0.23km2) </a:t>
+            <a:t>(0.23km2) </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>注</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>)</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ Ｐゴシック"/>
-              <a:ea typeface="ＭＳ Ｐゴシック"/>
-              <a:cs typeface="ＭＳ Ｐゴシック"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>一部境界未定のため，総務省統計局において推定した｡</a:t>
+            <a:t>一部境界未定のため，総務省統計局において推定した</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Calibri"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>｡</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US"/>
             <a:t> </a:t>
           </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ホワイト">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1589,12 +1472,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1624,12 +1507,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1691,16 +1574,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1822,46 +1709,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -1871,53 +1719,53 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="3" width="11.875" customWidth="1"/>
     <col min="4" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" thickBot="1"/>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A3" s="11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="B3" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="H3" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="I3" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1925,28 +1773,28 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7">
-        <v>5383579</v>
+        <v>5627737</v>
       </c>
       <c r="E4" s="9">
-        <v>5506419</v>
+        <v>5683062</v>
       </c>
       <c r="F4" s="7">
-        <v>-122840</v>
-      </c>
-      <c r="G4" s="23">
-        <v>-2.2308509395999998</v>
+        <v>-55325</v>
+      </c>
+      <c r="G4" s="9">
+        <v>-1</v>
       </c>
       <c r="H4" s="16">
-        <v>83424.22</v>
+        <v>83455.73</v>
       </c>
       <c r="I4" s="13">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+        <v>71.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1954,28 +1802,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2">
-        <v>1308649</v>
+        <v>1436657</v>
       </c>
       <c r="E5" s="3">
-        <v>1373339</v>
+        <v>1475728</v>
       </c>
       <c r="F5" s="2">
-        <v>-64690</v>
-      </c>
-      <c r="G5" s="24">
-        <v>-4.7104174570000001</v>
+        <v>-39071</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-2.6</v>
       </c>
       <c r="H5" s="17">
-        <v>9645.4</v>
+        <v>9606.8799999999992</v>
       </c>
       <c r="I5" s="14">
-        <v>135.69999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+        <v>149.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1983,28 +1831,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2">
-        <v>1279814</v>
+        <v>1385041</v>
       </c>
       <c r="E6" s="3">
-        <v>1330147</v>
+        <v>1416180</v>
       </c>
       <c r="F6" s="2">
-        <v>-50333</v>
-      </c>
-      <c r="G6" s="24">
-        <v>-3.7840178566999998</v>
+        <v>-31139</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H6" s="17">
-        <v>15275.01</v>
+        <v>15278.71</v>
       </c>
       <c r="I6" s="14">
-        <v>83.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2012,28 +1860,28 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2">
-        <v>2334215</v>
+        <v>2360218</v>
       </c>
       <c r="E7" s="3">
-        <v>2348165</v>
+        <v>2365320</v>
       </c>
       <c r="F7" s="2">
-        <v>-13950</v>
-      </c>
-      <c r="G7" s="24">
-        <v>-0.59408090999999996</v>
+        <v>-5102</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-0.2</v>
       </c>
       <c r="H7" s="17">
-        <v>7282.14</v>
+        <v>7285.6</v>
       </c>
       <c r="I7" s="14">
-        <v>320.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2041,28 +1889,28 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2">
-        <v>1022839</v>
+        <v>1145501</v>
       </c>
       <c r="E8" s="3">
-        <v>1085997</v>
+        <v>1189279</v>
       </c>
       <c r="F8" s="2">
-        <v>-63158</v>
-      </c>
-      <c r="G8" s="24">
-        <v>-5.8156698407</v>
+        <v>-43778</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-3.7</v>
       </c>
       <c r="H8" s="17">
-        <v>11637.54</v>
+        <v>11612.22</v>
       </c>
       <c r="I8" s="14">
-        <v>87.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2070,28 +1918,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2">
-        <v>1122957</v>
+        <v>1216181</v>
       </c>
       <c r="E9" s="3">
-        <v>1168924</v>
+        <v>1244147</v>
       </c>
       <c r="F9" s="2">
-        <v>-45967</v>
-      </c>
-      <c r="G9" s="24">
-        <v>-3.9324199006999998</v>
+        <v>-27966</v>
+      </c>
+      <c r="G9" s="3">
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H9" s="17">
-        <v>9323.15</v>
+        <v>9323.39</v>
       </c>
       <c r="I9" s="14">
-        <v>120.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+        <v>130.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -2099,28 +1947,28 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2">
-        <v>1913606</v>
+        <v>2091319</v>
       </c>
       <c r="E10" s="3">
-        <v>2029064</v>
+        <v>2126935</v>
       </c>
       <c r="F10" s="2">
-        <v>-115458</v>
-      </c>
-      <c r="G10" s="24">
-        <v>-5.6902098702000004</v>
+        <v>-35616</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-1.7</v>
       </c>
       <c r="H10" s="17">
-        <v>13783.75</v>
+        <v>13782.75</v>
       </c>
       <c r="I10" s="14">
-        <v>138.80000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+        <v>151.69999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -2128,28 +1976,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2">
-        <v>2917857</v>
+        <v>2975167</v>
       </c>
       <c r="E11" s="3">
-        <v>2969770</v>
+        <v>2985676</v>
       </c>
       <c r="F11" s="2">
-        <v>-51913</v>
-      </c>
-      <c r="G11" s="24">
-        <v>-1.7480478286000001</v>
+        <v>-10509</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-0.4</v>
       </c>
       <c r="H11" s="17">
-        <v>6096.93</v>
+        <v>6095.68</v>
       </c>
       <c r="I11" s="14">
-        <v>478.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+        <v>488.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2157,28 +2005,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2">
-        <v>1974671</v>
+        <v>2016631</v>
       </c>
       <c r="E12" s="3">
-        <v>2007683</v>
+        <v>2004817</v>
       </c>
       <c r="F12" s="2">
-        <v>-33012</v>
-      </c>
-      <c r="G12" s="24">
-        <v>-1.6442834850000001</v>
+        <v>11814</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.6</v>
       </c>
       <c r="H12" s="17">
-        <v>6408.09</v>
+        <v>6408.28</v>
       </c>
       <c r="I12" s="14">
-        <v>308.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+        <v>314.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2186,28 +2034,28 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2">
-        <v>1973476</v>
+        <v>2024135</v>
       </c>
       <c r="E13" s="3">
-        <v>2008068</v>
+        <v>2024852</v>
       </c>
       <c r="F13" s="2">
-        <v>-34592</v>
-      </c>
-      <c r="G13" s="24">
-        <v>-1.7226508266</v>
+        <v>-717</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
       </c>
       <c r="H13" s="17">
-        <v>6362.28</v>
+        <v>6363.16</v>
       </c>
       <c r="I13" s="14">
-        <v>310.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+        <v>318.10000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2215,28 +2063,28 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2">
-        <v>7261271</v>
+        <v>7054243</v>
       </c>
       <c r="E14" s="3">
-        <v>7194556</v>
+        <v>6938006</v>
       </c>
       <c r="F14" s="2">
-        <v>66715</v>
-      </c>
-      <c r="G14" s="24">
-        <v>0.9272983628</v>
+        <v>116237</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1.7</v>
       </c>
       <c r="H14" s="17">
-        <v>3797.75</v>
+        <v>3797.3</v>
       </c>
       <c r="I14" s="14">
-        <v>1912</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1857.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2244,28 +2092,28 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2">
-        <v>6224027</v>
+        <v>6056462</v>
       </c>
       <c r="E15" s="3">
-        <v>6216289</v>
+        <v>5926285</v>
       </c>
       <c r="F15" s="2">
-        <v>7738</v>
-      </c>
-      <c r="G15" s="24">
-        <v>0.12447941210000001</v>
+        <v>130177</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2.2000000000000002</v>
       </c>
       <c r="H15" s="17">
-        <v>5157.6400000000003</v>
+        <v>5156.68</v>
       </c>
       <c r="I15" s="14">
-        <v>1206.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1174.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2273,28 +2121,28 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2">
-        <v>13513734</v>
+        <v>12576601</v>
       </c>
       <c r="E16" s="3">
-        <v>13159417</v>
+        <v>12064143</v>
       </c>
       <c r="F16" s="2">
-        <v>354317</v>
-      </c>
-      <c r="G16" s="24">
-        <v>2.6924976996000001</v>
+        <v>512458</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4.2</v>
       </c>
       <c r="H16" s="17">
-        <v>2190.9</v>
+        <v>2186.96</v>
       </c>
       <c r="I16" s="14">
-        <v>6168.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+        <v>5750.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2302,28 +2150,28 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" s="2">
-        <v>9127323</v>
+        <v>8791597</v>
       </c>
       <c r="E17" s="3">
-        <v>9048302</v>
+        <v>8489932</v>
       </c>
       <c r="F17" s="2">
-        <v>79021</v>
-      </c>
-      <c r="G17" s="24">
-        <v>0.87332407779999999</v>
+        <v>301665</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3.6</v>
       </c>
       <c r="H17" s="17">
-        <v>2415.81</v>
+        <v>2415.84</v>
       </c>
       <c r="I17" s="14">
-        <v>3778.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+        <v>3639.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2331,28 +2179,28 @@
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2">
-        <v>2305098</v>
+        <v>2431459</v>
       </c>
       <c r="E18" s="3">
-        <v>2374450</v>
+        <v>2475733</v>
       </c>
       <c r="F18" s="2">
-        <v>-69352</v>
-      </c>
-      <c r="G18" s="24">
-        <v>-2.9207605972000001</v>
+        <v>-44274</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-1.8</v>
       </c>
       <c r="H18" s="17">
-        <v>12584.1</v>
+        <v>12583.32</v>
       </c>
       <c r="I18" s="14">
-        <v>183.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+        <v>193.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2360,28 +2208,28 @@
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2">
-        <v>1066883</v>
+        <v>1111729</v>
       </c>
       <c r="E19" s="3">
-        <v>1093247</v>
+        <v>1120851</v>
       </c>
       <c r="F19" s="2">
-        <v>-26364</v>
-      </c>
-      <c r="G19" s="24">
-        <v>-2.4115318862000001</v>
+        <v>-9122</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-0.8</v>
       </c>
       <c r="H19" s="17">
-        <v>4247.6099999999997</v>
+        <v>4247.3900000000003</v>
       </c>
       <c r="I19" s="14">
-        <v>251.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+        <v>261.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2389,28 +2237,28 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2">
-        <v>1154343</v>
+        <v>1174026</v>
       </c>
       <c r="E20" s="3">
-        <v>1169788</v>
+        <v>1180977</v>
       </c>
       <c r="F20" s="2">
-        <v>-15445</v>
-      </c>
-      <c r="G20" s="24">
-        <v>-1.3203247084</v>
+        <v>-6951</v>
+      </c>
+      <c r="G20" s="3">
+        <v>-0.6</v>
       </c>
       <c r="H20" s="17">
-        <v>4186.1499999999996</v>
+        <v>4185.46</v>
       </c>
       <c r="I20" s="14">
-        <v>275.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+        <v>280.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2418,28 +2266,28 @@
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2">
-        <v>787099</v>
+        <v>821592</v>
       </c>
       <c r="E21" s="3">
-        <v>806314</v>
+        <v>828944</v>
       </c>
       <c r="F21" s="2">
-        <v>-19215</v>
-      </c>
-      <c r="G21" s="24">
-        <v>-2.3830666465000001</v>
+        <v>-7352</v>
+      </c>
+      <c r="G21" s="3">
+        <v>-0.9</v>
       </c>
       <c r="H21" s="17">
-        <v>4190.43</v>
+        <v>4189.25</v>
       </c>
       <c r="I21" s="14">
-        <v>187.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+        <v>196.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2447,28 +2295,28 @@
         <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" s="2">
-        <v>835165</v>
+        <v>884515</v>
       </c>
       <c r="E22" s="3">
-        <v>863075</v>
+        <v>888172</v>
       </c>
       <c r="F22" s="2">
-        <v>-27910</v>
-      </c>
-      <c r="G22" s="24">
-        <v>-3.2337861714999998</v>
+        <v>-3657</v>
+      </c>
+      <c r="G22" s="3">
+        <v>-0.4</v>
       </c>
       <c r="H22" s="17">
-        <v>4464.99</v>
+        <v>4465.37</v>
       </c>
       <c r="I22" s="14">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+        <v>198.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2476,28 +2324,28 @@
         <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2">
-        <v>2099759</v>
+        <v>2196114</v>
       </c>
       <c r="E23" s="3">
-        <v>2152449</v>
+        <v>2213128</v>
       </c>
       <c r="F23" s="2">
-        <v>-52690</v>
-      </c>
-      <c r="G23" s="24">
-        <v>-2.4479093348999998</v>
+        <v>-17014</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-0.8</v>
       </c>
       <c r="H23" s="17">
-        <v>13561.56</v>
+        <v>13562.23</v>
       </c>
       <c r="I23" s="14">
-        <v>154.80000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+        <v>161.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -2505,28 +2353,28 @@
         <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2">
-        <v>2032533</v>
+        <v>2107226</v>
       </c>
       <c r="E24" s="3">
-        <v>2080773</v>
+        <v>2109740</v>
       </c>
       <c r="F24" s="2">
-        <v>-48240</v>
-      </c>
-      <c r="G24" s="24">
-        <v>-2.3183691830000002</v>
+        <v>-2514</v>
+      </c>
+      <c r="G24" s="3">
+        <v>-0.1</v>
       </c>
       <c r="H24" s="17">
-        <v>10621.29</v>
+        <v>10621.17</v>
       </c>
       <c r="I24" s="14">
-        <v>191.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+        <v>198.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -2534,28 +2382,28 @@
         <v>21</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2">
-        <v>3701181</v>
+        <v>3792377</v>
       </c>
       <c r="E25" s="3">
-        <v>3765007</v>
+        <v>3767393</v>
       </c>
       <c r="F25" s="2">
-        <v>-63826</v>
-      </c>
-      <c r="G25" s="24">
-        <v>-1.6952425321</v>
+        <v>24984</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.7</v>
       </c>
       <c r="H25" s="17">
-        <v>7778.7</v>
+        <v>7780.03</v>
       </c>
       <c r="I25" s="14">
-        <v>475.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+        <v>487.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2563,28 +2411,28 @@
         <v>22</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2">
-        <v>7484094</v>
+        <v>7254704</v>
       </c>
       <c r="E26" s="3">
-        <v>7410719</v>
+        <v>7043300</v>
       </c>
       <c r="F26" s="2">
-        <v>73375</v>
-      </c>
-      <c r="G26" s="24">
-        <v>0.99011985209999998</v>
+        <v>211404</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
       </c>
       <c r="H26" s="17">
-        <v>5172.3999999999996</v>
+        <v>5164.0200000000004</v>
       </c>
       <c r="I26" s="14">
-        <v>1446.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1404.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -2592,28 +2440,28 @@
         <v>23</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2">
-        <v>1815827</v>
+        <v>1866963</v>
       </c>
       <c r="E27" s="3">
-        <v>1854724</v>
+        <v>1857339</v>
       </c>
       <c r="F27" s="2">
-        <v>-38897</v>
-      </c>
-      <c r="G27" s="24">
-        <v>-2.0971853494000001</v>
+        <v>9624</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.5</v>
       </c>
       <c r="H27" s="17">
-        <v>5774.39</v>
+        <v>5776.68</v>
       </c>
       <c r="I27" s="14">
-        <v>314.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+        <v>323.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -2621,28 +2469,28 @@
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2">
-        <v>1413184</v>
+        <v>1380361</v>
       </c>
       <c r="E28" s="3">
-        <v>1410777</v>
+        <v>1342832</v>
       </c>
       <c r="F28" s="2">
-        <v>2407</v>
-      </c>
-      <c r="G28" s="24">
-        <v>0.17061519999999999</v>
+        <v>37529</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.8</v>
       </c>
       <c r="H28" s="17">
-        <v>4017.38</v>
+        <v>4017.36</v>
       </c>
       <c r="I28" s="14">
-        <v>351.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+        <v>343.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -2650,28 +2498,28 @@
         <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D29" s="2">
-        <v>2610140</v>
+        <v>2647660</v>
       </c>
       <c r="E29" s="3">
-        <v>2636092</v>
+        <v>2644391</v>
       </c>
       <c r="F29" s="2">
-        <v>-25952</v>
-      </c>
-      <c r="G29" s="24">
-        <v>-0.98448764310000003</v>
+        <v>3269</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.1</v>
       </c>
       <c r="H29" s="17">
-        <v>4612.2</v>
+        <v>4613</v>
       </c>
       <c r="I29" s="14">
-        <v>565.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2679,28 +2527,28 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D30" s="2">
-        <v>8838908</v>
+        <v>8817166</v>
       </c>
       <c r="E30" s="3">
-        <v>8865245</v>
+        <v>8805081</v>
       </c>
       <c r="F30" s="2">
-        <v>-26337</v>
-      </c>
-      <c r="G30" s="24">
-        <v>-0.29708146810000002</v>
+        <v>12085</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.1</v>
       </c>
       <c r="H30" s="17">
-        <v>1904.99</v>
+        <v>1894.31</v>
       </c>
       <c r="I30" s="14">
-        <v>4639.8999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+        <v>4654.6000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2708,28 +2556,28 @@
         <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D31" s="2">
-        <v>5536989</v>
+        <v>5590601</v>
       </c>
       <c r="E31" s="3">
-        <v>5588133</v>
+        <v>5550574</v>
       </c>
       <c r="F31" s="2">
-        <v>-51144</v>
-      </c>
-      <c r="G31" s="24">
-        <v>-0.91522517449999996</v>
+        <v>40027</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.7</v>
       </c>
       <c r="H31" s="17">
-        <v>8400.9</v>
+        <v>8394.92</v>
       </c>
       <c r="I31" s="14">
-        <v>659.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2737,28 +2585,28 @@
         <v>28</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2">
-        <v>1365008</v>
+        <v>1421310</v>
       </c>
       <c r="E32" s="3">
-        <v>1400728</v>
+        <v>1442795</v>
       </c>
       <c r="F32" s="2">
-        <v>-35720</v>
-      </c>
-      <c r="G32" s="24">
-        <v>-2.5501025181000001</v>
+        <v>-21485</v>
+      </c>
+      <c r="G32" s="3">
+        <v>-1.5</v>
       </c>
       <c r="H32" s="17">
-        <v>3690.94</v>
+        <v>3691.09</v>
       </c>
       <c r="I32" s="14">
-        <v>369.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+        <v>385.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2766,28 +2614,28 @@
         <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2">
-        <v>963850</v>
+        <v>1035969</v>
       </c>
       <c r="E33" s="3">
-        <v>1002198</v>
+        <v>1069912</v>
       </c>
       <c r="F33" s="2">
-        <v>-38348</v>
-      </c>
-      <c r="G33" s="24">
-        <v>-3.8263895956999998</v>
+        <v>-33943</v>
+      </c>
+      <c r="G33" s="3">
+        <v>-3.2</v>
       </c>
       <c r="H33" s="17">
-        <v>4724.68</v>
+        <v>4726.08</v>
       </c>
       <c r="I33" s="14">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+        <v>219.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2795,28 +2643,28 @@
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D34" s="2">
-        <v>573648</v>
+        <v>607012</v>
       </c>
       <c r="E34" s="3">
-        <v>588667</v>
+        <v>613289</v>
       </c>
       <c r="F34" s="2">
-        <v>-15019</v>
-      </c>
-      <c r="G34" s="24">
-        <v>-2.5513575586999999</v>
+        <v>-6277</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-1</v>
       </c>
       <c r="H34" s="17">
-        <v>3507.05</v>
+        <v>3507.25</v>
       </c>
       <c r="I34" s="14">
-        <v>163.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+        <v>173.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2824,28 +2672,28 @@
         <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D35" s="2">
-        <v>694188</v>
+        <v>742223</v>
       </c>
       <c r="E35" s="3">
-        <v>717397</v>
+        <v>761503</v>
       </c>
       <c r="F35" s="2">
-        <v>-23209</v>
-      </c>
-      <c r="G35" s="24">
-        <v>-3.2351682541</v>
+        <v>-19280</v>
+      </c>
+      <c r="G35" s="3">
+        <v>-2.5</v>
       </c>
       <c r="H35" s="17">
-        <v>6708.23</v>
+        <v>6707.56</v>
       </c>
       <c r="I35" s="14">
-        <v>103.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+        <v>110.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2853,28 +2701,28 @@
         <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D36" s="2">
-        <v>1922181</v>
+        <v>1957264</v>
       </c>
       <c r="E36" s="3">
-        <v>1945276</v>
+        <v>1950828</v>
       </c>
       <c r="F36" s="2">
-        <v>-23095</v>
-      </c>
-      <c r="G36" s="24">
-        <v>-1.1872351275999999</v>
+        <v>6436</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.3</v>
       </c>
       <c r="H36" s="17">
-        <v>7114.62</v>
+        <v>7112.73</v>
       </c>
       <c r="I36" s="14">
-        <v>270.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+        <v>275.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2882,28 +2730,28 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D37" s="2">
-        <v>2844963</v>
+        <v>2876642</v>
       </c>
       <c r="E37" s="3">
-        <v>2860750</v>
+        <v>2878915</v>
       </c>
       <c r="F37" s="2">
-        <v>-15787</v>
-      </c>
-      <c r="G37" s="24">
-        <v>-0.55184829150000003</v>
+        <v>-2273</v>
+      </c>
+      <c r="G37" s="3">
+        <v>-0.1</v>
       </c>
       <c r="H37" s="17">
-        <v>8479.3799999999992</v>
+        <v>8477.92</v>
       </c>
       <c r="I37" s="14">
-        <v>335.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+        <v>339.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2911,28 +2759,28 @@
         <v>34</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D38" s="2">
-        <v>1405007</v>
+        <v>1492606</v>
       </c>
       <c r="E38" s="3">
-        <v>1451338</v>
+        <v>1527964</v>
       </c>
       <c r="F38" s="2">
-        <v>-46331</v>
-      </c>
-      <c r="G38" s="24">
-        <v>-3.1922956610000002</v>
+        <v>-35358</v>
+      </c>
+      <c r="G38" s="3">
+        <v>-2.2999999999999998</v>
       </c>
       <c r="H38" s="17">
-        <v>6112.3</v>
+        <v>6111.91</v>
       </c>
       <c r="I38" s="14">
-        <v>229.9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+        <v>244.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2940,28 +2788,28 @@
         <v>35</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2">
-        <v>756063</v>
+        <v>809950</v>
       </c>
       <c r="E39" s="3">
-        <v>785491</v>
+        <v>824108</v>
       </c>
       <c r="F39" s="2">
-        <v>-29428</v>
-      </c>
-      <c r="G39" s="24">
-        <v>-3.7464464901999999</v>
+        <v>-14158</v>
+      </c>
+      <c r="G39" s="3">
+        <v>-1.7</v>
       </c>
       <c r="H39" s="17">
-        <v>4146.93</v>
+        <v>4145.33</v>
       </c>
       <c r="I39" s="14">
-        <v>182.3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+        <v>195.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2969,28 +2817,28 @@
         <v>36</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D40" s="2">
-        <v>976756</v>
+        <v>1012400</v>
       </c>
       <c r="E40" s="3">
-        <v>995842</v>
+        <v>1022890</v>
       </c>
       <c r="F40" s="2">
-        <v>-19086</v>
-      </c>
-      <c r="G40" s="24">
-        <v>-1.9165690943</v>
+        <v>-10490</v>
+      </c>
+      <c r="G40" s="3">
+        <v>-1</v>
       </c>
       <c r="H40" s="17">
-        <v>1876.73</v>
+        <v>1876.41</v>
       </c>
       <c r="I40" s="14">
-        <v>520.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+        <v>539.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2998,28 +2846,28 @@
         <v>37</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2">
-        <v>1385840</v>
+        <v>1467815</v>
       </c>
       <c r="E41" s="3">
-        <v>1431493</v>
+        <v>1493092</v>
       </c>
       <c r="F41" s="2">
-        <v>-45653</v>
-      </c>
-      <c r="G41" s="24">
-        <v>-3.1891877919999998</v>
+        <v>-25277</v>
+      </c>
+      <c r="G41" s="3">
+        <v>-1.7</v>
       </c>
       <c r="H41" s="17">
-        <v>5676.1</v>
+        <v>5677.12</v>
       </c>
       <c r="I41" s="14">
-        <v>244.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+        <v>258.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -3027,28 +2875,28 @@
         <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2">
-        <v>728461</v>
+        <v>796292</v>
       </c>
       <c r="E42" s="3">
-        <v>764456</v>
+        <v>813949</v>
       </c>
       <c r="F42" s="2">
-        <v>-35995</v>
-      </c>
-      <c r="G42" s="24">
-        <v>-4.7085770796000004</v>
+        <v>-17657</v>
+      </c>
+      <c r="G42" s="3">
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H42" s="17">
-        <v>7103.91</v>
+        <v>7105.01</v>
       </c>
       <c r="I42" s="14">
-        <v>102.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+        <v>112.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -3056,28 +2904,28 @@
         <v>39</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D43" s="2">
-        <v>5102871</v>
+        <v>5049908</v>
       </c>
       <c r="E43" s="3">
-        <v>5071968</v>
+        <v>5015699</v>
       </c>
       <c r="F43" s="2">
-        <v>30903</v>
-      </c>
-      <c r="G43" s="24">
-        <v>0.60929012169999996</v>
+        <v>34209</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.7</v>
       </c>
       <c r="H43" s="17">
-        <v>4986.3999999999996</v>
+        <v>4976.12</v>
       </c>
       <c r="I43" s="14">
-        <v>1023.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1014.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -3085,28 +2933,28 @@
         <v>40</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D44" s="2">
-        <v>833245</v>
+        <v>866369</v>
       </c>
       <c r="E44" s="3">
-        <v>849788</v>
+        <v>876654</v>
       </c>
       <c r="F44" s="2">
-        <v>-16543</v>
-      </c>
-      <c r="G44" s="24">
-        <v>-1.9467208292</v>
+        <v>-10285</v>
+      </c>
+      <c r="G44" s="3">
+        <v>-1.2</v>
       </c>
       <c r="H44" s="17">
-        <v>2440.64</v>
+        <v>2439.58</v>
       </c>
       <c r="I44" s="14">
-        <v>341.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+        <v>355.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -3114,28 +2962,28 @@
         <v>41</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D45" s="2">
-        <v>1377780</v>
+        <v>1478632</v>
       </c>
       <c r="E45" s="3">
-        <v>1426779</v>
+        <v>1516523</v>
       </c>
       <c r="F45" s="2">
-        <v>-48999</v>
-      </c>
-      <c r="G45" s="24">
-        <v>-3.4342389396000002</v>
+        <v>-37891</v>
+      </c>
+      <c r="G45" s="3">
+        <v>-2.5</v>
       </c>
       <c r="H45" s="17">
-        <v>4132.32</v>
+        <v>4094.76</v>
       </c>
       <c r="I45" s="14">
-        <v>333.4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+        <v>361.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -3143,28 +2991,28 @@
         <v>42</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D46" s="2">
-        <v>1786969</v>
+        <v>1842233</v>
       </c>
       <c r="E46" s="3">
-        <v>1817426</v>
+        <v>1859344</v>
       </c>
       <c r="F46" s="2">
-        <v>-30457</v>
-      </c>
-      <c r="G46" s="24">
-        <v>-1.6758316432</v>
+        <v>-17111</v>
+      </c>
+      <c r="G46" s="3">
+        <v>-0.9</v>
       </c>
       <c r="H46" s="17">
-        <v>7409.32</v>
+        <v>7404.83</v>
       </c>
       <c r="I46" s="14">
-        <v>241.2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+        <v>248.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -3172,28 +3020,28 @@
         <v>43</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D47" s="2">
-        <v>1166729</v>
+        <v>1209571</v>
       </c>
       <c r="E47" s="3">
-        <v>1196529</v>
+        <v>1221140</v>
       </c>
       <c r="F47" s="2">
-        <v>-29800</v>
-      </c>
-      <c r="G47" s="24">
-        <v>-2.4905372122</v>
+        <v>-11569</v>
+      </c>
+      <c r="G47" s="3">
+        <v>-0.9</v>
       </c>
       <c r="H47" s="17">
-        <v>6340.61</v>
+        <v>6339.32</v>
       </c>
       <c r="I47" s="14">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+        <v>190.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -3201,28 +3049,28 @@
         <v>44</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D48" s="2">
-        <v>1104377</v>
+        <v>1153042</v>
       </c>
       <c r="E48" s="3">
-        <v>1135233</v>
+        <v>1170007</v>
       </c>
       <c r="F48" s="2">
-        <v>-30856</v>
-      </c>
-      <c r="G48" s="24">
-        <v>-2.7180323335000001</v>
+        <v>-16965</v>
+      </c>
+      <c r="G48" s="3">
+        <v>-1.4</v>
       </c>
       <c r="H48" s="17">
-        <v>7735.31</v>
+        <v>7734.77</v>
       </c>
       <c r="I48" s="14">
-        <v>142.80000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+        <v>149.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -3230,28 +3078,28 @@
         <v>45</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D49" s="2">
-        <v>1648752</v>
+        <v>1753179</v>
       </c>
       <c r="E49" s="3">
-        <v>1706242</v>
+        <v>1786194</v>
       </c>
       <c r="F49" s="2">
-        <v>-57490</v>
-      </c>
-      <c r="G49" s="24">
-        <v>-3.3693930873000002</v>
+        <v>-33015</v>
+      </c>
+      <c r="G49" s="3">
+        <v>-1.8</v>
       </c>
       <c r="H49" s="17">
-        <v>9188.1</v>
+        <v>9187.69</v>
       </c>
       <c r="I49" s="14">
-        <v>179.4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+        <v>190.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="14.25" thickBot="1">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -3259,32 +3107,33 @@
         <v>46</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D50" s="4">
-        <v>1434138</v>
+        <v>1361594</v>
       </c>
       <c r="E50" s="6">
-        <v>1392818</v>
+        <v>1318220</v>
       </c>
       <c r="F50" s="4">
-        <v>41320</v>
-      </c>
-      <c r="G50" s="25">
-        <v>2.9666474730000001</v>
+        <v>43374</v>
+      </c>
+      <c r="G50" s="6">
+        <v>3.3</v>
       </c>
       <c r="H50" s="18">
-        <v>2281</v>
+        <v>2274.59</v>
       </c>
       <c r="I50" s="15">
-        <v>628.70000000000005</v>
+        <v>598.6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78700000000000003" right="0.78700000000000003" top="0.98399999999999999" bottom="0.98399999999999999" header="0.51200000000000001" footer="0.51200000000000001"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3294,10 +3143,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78700000000000003" right="0.78700000000000003" top="0.98399999999999999" bottom="0.98399999999999999" header="0.51200000000000001" footer="0.51200000000000001"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -3307,9 +3157,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78700000000000003" right="0.78700000000000003" top="0.98399999999999999" bottom="0.98399999999999999" header="0.51200000000000001" footer="0.51200000000000001"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>